<commit_message>
ajuste para procesar set de datos menor a 24
</commit_message>
<xml_diff>
--- a/dataset/plantilla_historico_codigo_cliente.xlsx
+++ b/dataset/plantilla_historico_codigo_cliente.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wilfe\Local_files\Python\Milagros\dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB4EFEFC-51F9-41D8-848B-1D9F24BAF90E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C3787F5-CF19-431B-9A80-C5F595FC8BA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="45972" yWindow="2868" windowWidth="30936" windowHeight="12456" xr2:uid="{D064CDE1-EB50-4886-8B37-32134DE54DB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AK$123</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -37,12 +40,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="131">
-  <si>
-    <t>CODIGO</t>
-  </si>
-  <si>
-    <t>DESCRIPCION</t>
-  </si>
   <si>
     <t>CLIENTE</t>
   </si>
@@ -429,6 +426,12 @@
   </si>
   <si>
     <t>AMPOLLETA ELIXIR</t>
+  </si>
+  <si>
+    <t>CODIGO</t>
+  </si>
+  <si>
+    <t>DESCRIPCION</t>
   </si>
 </sst>
 </file>
@@ -886,10 +889,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{448F5820-9B09-4170-A743-862EF891E4AC}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:AK123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D128" sqref="D128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -933,128 +937,128 @@
     <col min="37" max="37" width="8.86328125" style="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:37" ht="17.5" customHeight="1" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>129</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AD1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AK1" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>37</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="D2" s="7">
         <v>0</v>
@@ -1161,13 +1165,13 @@
     </row>
     <row r="3" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A3" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="D3" s="8">
         <v>0</v>
@@ -1256,7 +1260,9 @@
       <c r="AF3" s="7">
         <v>0</v>
       </c>
-      <c r="AG3" s="7"/>
+      <c r="AG3" s="7">
+        <v>0</v>
+      </c>
       <c r="AH3" s="7">
         <v>2</v>
       </c>
@@ -1270,15 +1276,15 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="4" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A4" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D4" s="7">
         <v>0</v>
@@ -1383,15 +1389,15 @@
         <v>23490</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="5" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>41</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="D5" s="7">
         <v>0</v>
@@ -1496,15 +1502,15 @@
         <v>2370</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="6" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A6" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>44</v>
       </c>
       <c r="D6" s="7">
         <v>0</v>
@@ -1609,15 +1615,15 @@
         <v>225</v>
       </c>
     </row>
-    <row r="7" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="7" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A7" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="8">
         <v>0</v>
@@ -1722,15 +1728,15 @@
         <v>39448</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="8" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A8" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D8" s="7">
         <v>0</v>
@@ -1835,15 +1841,15 @@
         <v>16020</v>
       </c>
     </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="9" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A9" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" s="7">
         <v>0</v>
@@ -1948,15 +1954,15 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="10" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A10" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D10" s="7">
         <v>0</v>
@@ -2061,15 +2067,15 @@
         <v>240</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="11" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A11" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D11" s="8">
         <v>6453</v>
@@ -2174,15 +2180,15 @@
         <v>97385</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="12" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A12" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D12" s="8">
         <v>0</v>
@@ -2287,15 +2293,15 @@
         <v>4112</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="13" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A13" s="5" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D13" s="7">
         <v>0</v>
@@ -2400,15 +2406,15 @@
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="14" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A14" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D14" s="8">
         <v>0</v>
@@ -2513,15 +2519,15 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="15" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A15" s="5" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D15" s="7">
         <v>0</v>
@@ -2626,15 +2632,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="16" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D16" s="8">
         <v>170</v>
@@ -2739,15 +2745,15 @@
         <v>1652</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="17" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A17" s="5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D17" s="7">
         <v>0</v>
@@ -2852,15 +2858,15 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="18" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A18" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D18" s="8">
         <v>250</v>
@@ -2965,15 +2971,15 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="19" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A19" s="5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D19" s="7">
         <v>0</v>
@@ -3078,15 +3084,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="20" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A20" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="7">
         <v>0</v>
@@ -3191,15 +3197,15 @@
         <v>14100</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="21" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A21" s="5" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D21" s="7">
         <v>0</v>
@@ -3304,15 +3310,15 @@
         <v>4175</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="22" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A22" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="8">
         <v>2905</v>
@@ -3417,15 +3423,15 @@
         <v>42113</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="23" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A23" s="5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D23" s="7">
         <v>0</v>
@@ -3530,15 +3536,15 @@
         <v>180</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="24" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A24" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D24" s="7">
         <v>0</v>
@@ -3643,15 +3649,15 @@
         <v>4860</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="25" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A25" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D25" s="7">
         <v>0</v>
@@ -3756,15 +3762,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="26" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A26" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D26" s="8">
         <v>0</v>
@@ -3869,15 +3875,15 @@
         <v>18184</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="27" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A27" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="8">
         <v>0</v>
@@ -3982,128 +3988,128 @@
         <v>3724</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="28" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A28" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="7">
+        <v>0</v>
+      </c>
+      <c r="E28" s="7">
+        <v>0</v>
+      </c>
+      <c r="F28" s="7">
+        <v>0</v>
+      </c>
+      <c r="G28" s="7">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7">
+        <v>0</v>
+      </c>
+      <c r="I28" s="7">
+        <v>0</v>
+      </c>
+      <c r="J28" s="7">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7">
+        <v>0</v>
+      </c>
+      <c r="L28" s="7">
+        <v>0</v>
+      </c>
+      <c r="M28" s="7">
+        <v>0</v>
+      </c>
+      <c r="N28" s="7">
+        <v>0</v>
+      </c>
+      <c r="O28" s="7">
+        <v>0</v>
+      </c>
+      <c r="P28" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="7">
+        <v>0</v>
+      </c>
+      <c r="R28" s="7">
+        <v>0</v>
+      </c>
+      <c r="S28" s="7">
+        <v>0</v>
+      </c>
+      <c r="T28" s="7">
+        <v>0</v>
+      </c>
+      <c r="U28" s="7">
+        <v>0</v>
+      </c>
+      <c r="V28" s="7">
+        <v>0</v>
+      </c>
+      <c r="W28" s="7">
+        <v>0</v>
+      </c>
+      <c r="X28" s="7">
+        <v>0</v>
+      </c>
+      <c r="Y28" s="7">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AH28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AI28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ28" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK28" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
+      <c r="A29" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B29" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D28" s="7">
-        <v>0</v>
-      </c>
-      <c r="E28" s="7">
-        <v>0</v>
-      </c>
-      <c r="F28" s="7">
-        <v>0</v>
-      </c>
-      <c r="G28" s="7">
-        <v>0</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0</v>
-      </c>
-      <c r="I28" s="7">
-        <v>0</v>
-      </c>
-      <c r="J28" s="7">
-        <v>0</v>
-      </c>
-      <c r="K28" s="7">
-        <v>0</v>
-      </c>
-      <c r="L28" s="7">
-        <v>0</v>
-      </c>
-      <c r="M28" s="7">
-        <v>0</v>
-      </c>
-      <c r="N28" s="7">
-        <v>0</v>
-      </c>
-      <c r="O28" s="7">
-        <v>0</v>
-      </c>
-      <c r="P28" s="7">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="7">
-        <v>0</v>
-      </c>
-      <c r="R28" s="7">
-        <v>0</v>
-      </c>
-      <c r="S28" s="7">
-        <v>0</v>
-      </c>
-      <c r="T28" s="7">
-        <v>0</v>
-      </c>
-      <c r="U28" s="7">
-        <v>0</v>
-      </c>
-      <c r="V28" s="7">
-        <v>0</v>
-      </c>
-      <c r="W28" s="7">
-        <v>0</v>
-      </c>
-      <c r="X28" s="7">
-        <v>0</v>
-      </c>
-      <c r="Y28" s="7">
-        <v>0</v>
-      </c>
-      <c r="Z28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AB28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AC28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AD28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AE28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AF28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AG28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AH28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AI28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ28" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK28" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.75">
-      <c r="A29" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="C29" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D29" s="7">
         <v>0</v>
@@ -4208,15 +4214,15 @@
         <v>1560</v>
       </c>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="30" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A30" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D30" s="7">
         <v>0</v>
@@ -4321,15 +4327,15 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="31" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A31" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D31" s="8">
         <v>0</v>
@@ -4434,15 +4440,15 @@
         <v>9438</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="32" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A32" s="10" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D32" s="8">
         <v>0</v>
@@ -4547,15 +4553,15 @@
         <v>4862</v>
       </c>
     </row>
-    <row r="33" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A33" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D33" s="7">
         <v>0</v>
@@ -4660,15 +4666,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="34" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A34" s="10" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D34" s="8">
         <v>0</v>
@@ -4773,15 +4779,15 @@
         <v>2130</v>
       </c>
     </row>
-    <row r="35" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="35" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A35" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D35" s="7">
         <v>0</v>
@@ -4886,15 +4892,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="36" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A36" s="10" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D36" s="8">
         <v>0</v>
@@ -4999,15 +5005,15 @@
         <v>2423</v>
       </c>
     </row>
-    <row r="37" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="37" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A37" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D37" s="7">
         <v>0</v>
@@ -5112,15 +5118,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="38" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="38" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A38" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D38" s="8">
         <v>0</v>
@@ -5225,15 +5231,15 @@
         <v>3185</v>
       </c>
     </row>
-    <row r="39" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="39" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A39" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D39" s="7">
         <v>0</v>
@@ -5338,15 +5344,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="40" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A40" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D40" s="7">
         <v>0</v>
@@ -5451,15 +5457,15 @@
         <v>7860</v>
       </c>
     </row>
-    <row r="41" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="41" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A41" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D41" s="7">
         <v>0</v>
@@ -5564,15 +5570,15 @@
         <v>16</v>
       </c>
     </row>
-    <row r="42" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="42" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A42" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D42" s="8">
         <v>0</v>
@@ -5677,15 +5683,15 @@
         <v>8227</v>
       </c>
     </row>
-    <row r="43" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="43" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A43" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D43" s="8">
         <v>0</v>
@@ -5790,15 +5796,15 @@
         <v>2886</v>
       </c>
     </row>
-    <row r="44" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="44" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A44" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D44" s="7">
         <v>0</v>
@@ -5903,15 +5909,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="45" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A45" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D45" s="7">
         <v>0</v>
@@ -6016,15 +6022,15 @@
         <v>9160</v>
       </c>
     </row>
-    <row r="46" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="46" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A46" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D46" s="7">
         <v>0</v>
@@ -6129,15 +6135,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="47" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="47" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A47" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D47" s="8">
         <v>2600</v>
@@ -6242,15 +6248,15 @@
         <v>25865</v>
       </c>
     </row>
-    <row r="48" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="48" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A48" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D48" s="7">
         <v>0</v>
@@ -6355,15 +6361,15 @@
         <v>13272</v>
       </c>
     </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A49" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D49" s="7">
         <v>0</v>
@@ -6468,15 +6474,15 @@
         <v>2304</v>
       </c>
     </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="50" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A50" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D50" s="7">
         <v>0</v>
@@ -6581,15 +6587,15 @@
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="51" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A51" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D51" s="8">
         <v>0</v>
@@ -6694,15 +6700,15 @@
         <v>11773</v>
       </c>
     </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="52" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A52" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D52" s="7">
         <v>0</v>
@@ -6807,15 +6813,15 @@
         <v>18020</v>
       </c>
     </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="53" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A53" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D53" s="8">
         <v>0</v>
@@ -6920,15 +6926,15 @@
         <v>201</v>
       </c>
     </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="54" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A54" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D54" s="7">
         <v>0</v>
@@ -7033,15 +7039,15 @@
         <v>6390</v>
       </c>
     </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="55" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A55" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D55" s="7">
         <v>0</v>
@@ -7146,15 +7152,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="56" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A56" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D56" s="8">
         <v>0</v>
@@ -7259,15 +7265,15 @@
         <v>6802</v>
       </c>
     </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="57" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A57" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D57" s="7">
         <v>0</v>
@@ -7372,15 +7378,15 @@
         <v>4200</v>
       </c>
     </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="58" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A58" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D58" s="7">
         <v>0</v>
@@ -7485,15 +7491,15 @@
         <v>1170</v>
       </c>
     </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="59" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A59" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D59" s="7">
         <v>0</v>
@@ -7598,15 +7604,15 @@
         <v>14040</v>
       </c>
     </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="60" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A60" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D60" s="7">
         <v>0</v>
@@ -7711,15 +7717,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="61" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A61" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D61" s="8">
         <v>0</v>
@@ -7824,15 +7830,15 @@
         <v>5336</v>
       </c>
     </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="62" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A62" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D62" s="8">
         <v>0</v>
@@ -7937,15 +7943,15 @@
         <v>4092</v>
       </c>
     </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="63" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A63" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D63" s="7">
         <v>0</v>
@@ -8050,15 +8056,15 @@
         <v>13</v>
       </c>
     </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="64" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A64" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D64" s="8">
         <v>0</v>
@@ -8163,15 +8169,15 @@
         <v>6745</v>
       </c>
     </row>
-    <row r="65" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="65" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A65" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D65" s="7">
         <v>0</v>
@@ -8276,15 +8282,15 @@
         <v>23</v>
       </c>
     </row>
-    <row r="66" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="66" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A66" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D66" s="8">
         <v>0</v>
@@ -8389,354 +8395,354 @@
         <v>23487</v>
       </c>
     </row>
-    <row r="67" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="67" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A67" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D67" s="7">
+        <v>0</v>
+      </c>
+      <c r="E67" s="7">
+        <v>0</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0</v>
+      </c>
+      <c r="G67" s="7">
+        <v>0</v>
+      </c>
+      <c r="H67" s="7">
+        <v>0</v>
+      </c>
+      <c r="I67" s="7">
+        <v>0</v>
+      </c>
+      <c r="J67" s="7">
+        <v>0</v>
+      </c>
+      <c r="K67" s="7">
+        <v>0</v>
+      </c>
+      <c r="L67" s="7">
+        <v>0</v>
+      </c>
+      <c r="M67" s="7">
+        <v>0</v>
+      </c>
+      <c r="N67" s="7">
+        <v>0</v>
+      </c>
+      <c r="O67" s="8">
+        <v>0</v>
+      </c>
+      <c r="P67" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q67" s="8">
+        <v>0</v>
+      </c>
+      <c r="R67" s="8">
+        <v>0</v>
+      </c>
+      <c r="S67" s="8">
+        <v>0</v>
+      </c>
+      <c r="T67" s="8">
+        <v>0</v>
+      </c>
+      <c r="U67" s="8">
+        <v>0</v>
+      </c>
+      <c r="V67" s="8">
+        <v>0</v>
+      </c>
+      <c r="W67" s="8">
+        <v>0</v>
+      </c>
+      <c r="X67" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y67" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH67" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ67" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK67" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
+      <c r="A68" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D68" s="7">
+        <v>0</v>
+      </c>
+      <c r="E68" s="7">
+        <v>0</v>
+      </c>
+      <c r="F68" s="7">
+        <v>0</v>
+      </c>
+      <c r="G68" s="7">
+        <v>0</v>
+      </c>
+      <c r="H68" s="7">
+        <v>0</v>
+      </c>
+      <c r="I68" s="7">
+        <v>0</v>
+      </c>
+      <c r="J68" s="7">
+        <v>0</v>
+      </c>
+      <c r="K68" s="7">
+        <v>0</v>
+      </c>
+      <c r="L68" s="7">
+        <v>0</v>
+      </c>
+      <c r="M68" s="7">
+        <v>0</v>
+      </c>
+      <c r="N68" s="7">
+        <v>0</v>
+      </c>
+      <c r="O68" s="8">
+        <v>0</v>
+      </c>
+      <c r="P68" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q68" s="8">
+        <v>0</v>
+      </c>
+      <c r="R68" s="8">
+        <v>0</v>
+      </c>
+      <c r="S68" s="8">
+        <v>0</v>
+      </c>
+      <c r="T68" s="8">
+        <v>0</v>
+      </c>
+      <c r="U68" s="8">
+        <v>0</v>
+      </c>
+      <c r="V68" s="8">
+        <v>0</v>
+      </c>
+      <c r="W68" s="8">
+        <v>0</v>
+      </c>
+      <c r="X68" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y68" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH68" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ68" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK68" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
+      <c r="A69" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D69" s="7">
+        <v>0</v>
+      </c>
+      <c r="E69" s="7">
+        <v>0</v>
+      </c>
+      <c r="F69" s="7">
+        <v>0</v>
+      </c>
+      <c r="G69" s="7">
+        <v>0</v>
+      </c>
+      <c r="H69" s="7">
+        <v>0</v>
+      </c>
+      <c r="I69" s="7">
+        <v>0</v>
+      </c>
+      <c r="J69" s="7">
+        <v>0</v>
+      </c>
+      <c r="K69" s="7">
+        <v>0</v>
+      </c>
+      <c r="L69" s="7">
+        <v>0</v>
+      </c>
+      <c r="M69" s="7">
+        <v>0</v>
+      </c>
+      <c r="N69" s="7">
+        <v>0</v>
+      </c>
+      <c r="O69" s="8">
+        <v>0</v>
+      </c>
+      <c r="P69" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q69" s="8">
+        <v>0</v>
+      </c>
+      <c r="R69" s="8">
+        <v>0</v>
+      </c>
+      <c r="S69" s="8">
+        <v>0</v>
+      </c>
+      <c r="T69" s="8">
+        <v>0</v>
+      </c>
+      <c r="U69" s="8">
+        <v>0</v>
+      </c>
+      <c r="V69" s="8">
+        <v>0</v>
+      </c>
+      <c r="W69" s="8">
+        <v>0</v>
+      </c>
+      <c r="X69" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y69" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH69" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AJ69" s="7">
+        <v>0</v>
+      </c>
+      <c r="AK69" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
+      <c r="A70" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B67" s="6" t="s">
+      <c r="B70" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="C67" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D67" s="7">
-        <v>0</v>
-      </c>
-      <c r="E67" s="7">
-        <v>0</v>
-      </c>
-      <c r="F67" s="7">
-        <v>0</v>
-      </c>
-      <c r="G67" s="7">
-        <v>0</v>
-      </c>
-      <c r="H67" s="7">
-        <v>0</v>
-      </c>
-      <c r="I67" s="7">
-        <v>0</v>
-      </c>
-      <c r="J67" s="7">
-        <v>0</v>
-      </c>
-      <c r="K67" s="7">
-        <v>0</v>
-      </c>
-      <c r="L67" s="7">
-        <v>0</v>
-      </c>
-      <c r="M67" s="7">
-        <v>0</v>
-      </c>
-      <c r="N67" s="7">
-        <v>0</v>
-      </c>
-      <c r="O67" s="8">
-        <v>0</v>
-      </c>
-      <c r="P67" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q67" s="8">
-        <v>0</v>
-      </c>
-      <c r="R67" s="8">
-        <v>0</v>
-      </c>
-      <c r="S67" s="8">
-        <v>0</v>
-      </c>
-      <c r="T67" s="8">
-        <v>0</v>
-      </c>
-      <c r="U67" s="8">
-        <v>0</v>
-      </c>
-      <c r="V67" s="8">
-        <v>0</v>
-      </c>
-      <c r="W67" s="8">
-        <v>0</v>
-      </c>
-      <c r="X67" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y67" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH67" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI67" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ67" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK67" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:37" x14ac:dyDescent="0.75">
-      <c r="A68" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D68" s="7">
-        <v>0</v>
-      </c>
-      <c r="E68" s="7">
-        <v>0</v>
-      </c>
-      <c r="F68" s="7">
-        <v>0</v>
-      </c>
-      <c r="G68" s="7">
-        <v>0</v>
-      </c>
-      <c r="H68" s="7">
-        <v>0</v>
-      </c>
-      <c r="I68" s="7">
-        <v>0</v>
-      </c>
-      <c r="J68" s="7">
-        <v>0</v>
-      </c>
-      <c r="K68" s="7">
-        <v>0</v>
-      </c>
-      <c r="L68" s="7">
-        <v>0</v>
-      </c>
-      <c r="M68" s="7">
-        <v>0</v>
-      </c>
-      <c r="N68" s="7">
-        <v>0</v>
-      </c>
-      <c r="O68" s="8">
-        <v>0</v>
-      </c>
-      <c r="P68" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q68" s="8">
-        <v>0</v>
-      </c>
-      <c r="R68" s="8">
-        <v>0</v>
-      </c>
-      <c r="S68" s="8">
-        <v>0</v>
-      </c>
-      <c r="T68" s="8">
-        <v>0</v>
-      </c>
-      <c r="U68" s="8">
-        <v>0</v>
-      </c>
-      <c r="V68" s="8">
-        <v>0</v>
-      </c>
-      <c r="W68" s="8">
-        <v>0</v>
-      </c>
-      <c r="X68" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y68" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH68" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI68" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ68" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK68" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:37" x14ac:dyDescent="0.75">
-      <c r="A69" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="C69" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="D69" s="7">
-        <v>0</v>
-      </c>
-      <c r="E69" s="7">
-        <v>0</v>
-      </c>
-      <c r="F69" s="7">
-        <v>0</v>
-      </c>
-      <c r="G69" s="7">
-        <v>0</v>
-      </c>
-      <c r="H69" s="7">
-        <v>0</v>
-      </c>
-      <c r="I69" s="7">
-        <v>0</v>
-      </c>
-      <c r="J69" s="7">
-        <v>0</v>
-      </c>
-      <c r="K69" s="7">
-        <v>0</v>
-      </c>
-      <c r="L69" s="7">
-        <v>0</v>
-      </c>
-      <c r="M69" s="7">
-        <v>0</v>
-      </c>
-      <c r="N69" s="7">
-        <v>0</v>
-      </c>
-      <c r="O69" s="8">
-        <v>0</v>
-      </c>
-      <c r="P69" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q69" s="8">
-        <v>0</v>
-      </c>
-      <c r="R69" s="8">
-        <v>0</v>
-      </c>
-      <c r="S69" s="8">
-        <v>0</v>
-      </c>
-      <c r="T69" s="8">
-        <v>0</v>
-      </c>
-      <c r="U69" s="8">
-        <v>0</v>
-      </c>
-      <c r="V69" s="8">
-        <v>0</v>
-      </c>
-      <c r="W69" s="8">
-        <v>0</v>
-      </c>
-      <c r="X69" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y69" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH69" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI69" s="7">
-        <v>0</v>
-      </c>
-      <c r="AJ69" s="7">
-        <v>0</v>
-      </c>
-      <c r="AK69" s="7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:37" x14ac:dyDescent="0.75">
-      <c r="A70" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B70" s="6" t="s">
-        <v>96</v>
-      </c>
       <c r="C70" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D70" s="7">
         <v>0</v>
@@ -8841,15 +8847,15 @@
         <v>2376</v>
       </c>
     </row>
-    <row r="71" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="71" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A71" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D71" s="7">
         <v>0</v>
@@ -8954,15 +8960,15 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="72" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A72" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C72" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D72" s="8">
         <v>0</v>
@@ -9067,15 +9073,15 @@
         <v>6535</v>
       </c>
     </row>
-    <row r="73" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="73" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A73" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D73" s="7">
         <v>0</v>
@@ -9180,15 +9186,15 @@
         <v>684</v>
       </c>
     </row>
-    <row r="74" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="74" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A74" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C74" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D74" s="7">
         <v>0</v>
@@ -9293,15 +9299,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="75" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="75" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A75" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C75" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D75" s="8">
         <v>0</v>
@@ -9408,13 +9414,13 @@
     </row>
     <row r="76" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A76" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C76" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D76" s="7">
         <v>0</v>
@@ -9521,13 +9527,13 @@
     </row>
     <row r="77" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A77" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C77" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D77" s="7">
         <v>0</v>
@@ -9634,13 +9640,13 @@
     </row>
     <row r="78" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A78" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C78" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D78" s="7">
         <v>0</v>
@@ -9747,13 +9753,13 @@
     </row>
     <row r="79" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A79" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C79" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D79" s="8">
         <v>0</v>
@@ -9824,13 +9830,27 @@
       <c r="Z79" s="7">
         <v>10536</v>
       </c>
-      <c r="AA79" s="7"/>
-      <c r="AB79" s="7"/>
-      <c r="AC79" s="7"/>
-      <c r="AD79" s="7"/>
-      <c r="AE79" s="7"/>
-      <c r="AF79" s="7"/>
-      <c r="AG79" s="7"/>
+      <c r="AA79" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB79" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC79" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD79" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE79" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF79" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG79" s="7">
+        <v>0</v>
+      </c>
       <c r="AH79" s="7">
         <v>29891</v>
       </c>
@@ -9844,15 +9864,15 @@
         <v>110725</v>
       </c>
     </row>
-    <row r="80" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="80" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A80" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C80" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D80" s="7">
         <v>0</v>
@@ -9957,15 +9977,15 @@
         <v>2760</v>
       </c>
     </row>
-    <row r="81" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="81" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A81" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C81" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D81" s="7">
         <v>0</v>
@@ -10070,15 +10090,15 @@
         <v>26</v>
       </c>
     </row>
-    <row r="82" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="82" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A82" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D82" s="8">
         <v>0</v>
@@ -10183,15 +10203,15 @@
         <v>4683</v>
       </c>
     </row>
-    <row r="83" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="83" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A83" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D83" s="8">
         <v>940</v>
@@ -10296,15 +10316,15 @@
         <v>35846</v>
       </c>
     </row>
-    <row r="84" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="84" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A84" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D84" s="7">
         <v>0</v>
@@ -10409,15 +10429,15 @@
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="85" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A85" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D85" s="8">
         <v>2625</v>
@@ -10522,15 +10542,15 @@
         <v>13186</v>
       </c>
     </row>
-    <row r="86" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="86" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A86" s="5" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C86" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D86" s="7">
         <v>0</v>
@@ -10637,13 +10657,13 @@
     </row>
     <row r="87" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A87" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C87" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D87" s="7">
         <v>0</v>
@@ -10750,13 +10770,13 @@
     </row>
     <row r="88" spans="1:37" x14ac:dyDescent="0.75">
       <c r="A88" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D88" s="8">
         <v>0</v>
@@ -10827,13 +10847,27 @@
       <c r="Z88" s="7">
         <v>13</v>
       </c>
-      <c r="AA88" s="7"/>
-      <c r="AB88" s="7"/>
-      <c r="AC88" s="7"/>
-      <c r="AD88" s="7"/>
-      <c r="AE88" s="7"/>
-      <c r="AF88" s="7"/>
-      <c r="AG88" s="7"/>
+      <c r="AA88" s="7">
+        <v>0</v>
+      </c>
+      <c r="AB88" s="7">
+        <v>0</v>
+      </c>
+      <c r="AC88" s="7">
+        <v>0</v>
+      </c>
+      <c r="AD88" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE88" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF88" s="7">
+        <v>0</v>
+      </c>
+      <c r="AG88" s="7">
+        <v>0</v>
+      </c>
       <c r="AH88" s="7">
         <v>1</v>
       </c>
@@ -10847,15 +10881,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="89" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="89" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A89" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C89" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D89" s="7">
         <v>0</v>
@@ -10960,15 +10994,15 @@
         <v>11580</v>
       </c>
     </row>
-    <row r="90" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="90" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A90" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C90" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D90" s="7">
         <v>0</v>
@@ -11073,15 +11107,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="91" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="91" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A91" s="5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D91" s="8">
         <v>6449</v>
@@ -11186,15 +11220,15 @@
         <v>57620</v>
       </c>
     </row>
-    <row r="92" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="92" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A92" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C92" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D92" s="8">
         <v>2955</v>
@@ -11299,15 +11333,15 @@
         <v>13958</v>
       </c>
     </row>
-    <row r="93" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="93" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A93" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C93" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D93" s="7">
         <v>0</v>
@@ -11412,15 +11446,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="94" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="94" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A94" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C94" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D94" s="7">
         <v>0</v>
@@ -11525,15 +11559,15 @@
         <v>32970</v>
       </c>
     </row>
-    <row r="95" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="95" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A95" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C95" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D95" s="7">
         <v>0</v>
@@ -11638,15 +11672,15 @@
         <v>4860</v>
       </c>
     </row>
-    <row r="96" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="96" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A96" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C96" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D96" s="7">
         <v>0</v>
@@ -11751,15 +11785,15 @@
         <v>207</v>
       </c>
     </row>
-    <row r="97" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="97" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A97" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C97" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D97" s="8">
         <v>0</v>
@@ -11864,15 +11898,15 @@
         <v>106766</v>
       </c>
     </row>
-    <row r="98" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="98" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A98" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D98" s="7">
         <v>0</v>
@@ -11977,15 +12011,15 @@
         <v>29</v>
       </c>
     </row>
-    <row r="99" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="99" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A99" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D99" s="7">
         <v>0</v>
@@ -12090,15 +12124,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="100" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A100" s="5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C100" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D100" s="8">
         <v>2465</v>
@@ -12203,15 +12237,15 @@
         <v>18008</v>
       </c>
     </row>
-    <row r="101" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="101" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A101" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C101" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D101" s="7">
         <v>0</v>
@@ -12316,15 +12350,15 @@
         <v>9600</v>
       </c>
     </row>
-    <row r="102" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="102" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A102" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C102" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D102" s="7">
         <v>0</v>
@@ -12429,15 +12463,15 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="103" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="103" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A103" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D103" s="7">
         <v>0</v>
@@ -12542,15 +12576,15 @@
         <v>106</v>
       </c>
     </row>
-    <row r="104" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="104" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A104" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C104" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D104" s="8">
         <v>0</v>
@@ -12655,15 +12689,15 @@
         <v>46232</v>
       </c>
     </row>
-    <row r="105" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="105" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A105" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C105" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D105" s="8">
         <v>1740</v>
@@ -12768,15 +12802,15 @@
         <v>11435</v>
       </c>
     </row>
-    <row r="106" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="106" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A106" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C106" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D106" s="7">
         <v>0</v>
@@ -12881,15 +12915,15 @@
         <v>30</v>
       </c>
     </row>
-    <row r="107" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="107" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A107" s="5" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C107" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D107" s="7">
         <v>0</v>
@@ -12994,15 +13028,15 @@
         <v>91</v>
       </c>
     </row>
-    <row r="108" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="108" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A108" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C108" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D108" s="8">
         <v>2915</v>
@@ -13107,15 +13141,15 @@
         <v>36062</v>
       </c>
     </row>
-    <row r="109" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="109" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A109" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C109" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D109" s="7">
         <v>0</v>
@@ -13220,15 +13254,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="110" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A110" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C110" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D110" s="7">
         <v>0</v>
@@ -13333,15 +13367,15 @@
         <v>99</v>
       </c>
     </row>
-    <row r="111" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="111" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A111" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C111" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D111" s="8">
         <v>1775</v>
@@ -13446,15 +13480,15 @@
         <v>28270</v>
       </c>
     </row>
-    <row r="112" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="112" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A112" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C112" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D112" s="7">
         <v>0</v>
@@ -13559,15 +13593,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="113" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="113" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A113" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C113" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D113" s="7">
         <v>0</v>
@@ -13672,15 +13706,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="114" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="114" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A114" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C114" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D114" s="7">
         <v>0</v>
@@ -13785,15 +13819,15 @@
         <v>6300</v>
       </c>
     </row>
-    <row r="115" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="115" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A115" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C115" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D115" s="7">
         <v>0</v>
@@ -13898,15 +13932,15 @@
         <v>103</v>
       </c>
     </row>
-    <row r="116" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="116" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A116" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C116" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D116" s="8">
         <v>0</v>
@@ -14011,15 +14045,15 @@
         <v>23792</v>
       </c>
     </row>
-    <row r="117" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="117" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A117" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C117" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D117" s="7">
         <v>0</v>
@@ -14124,15 +14158,15 @@
         <v>1860</v>
       </c>
     </row>
-    <row r="118" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="118" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A118" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C118" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D118" s="7">
         <v>0</v>
@@ -14237,15 +14271,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="119" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="119" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A119" s="5" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C119" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D119" s="8">
         <v>1719</v>
@@ -14350,15 +14384,15 @@
         <v>29118</v>
       </c>
     </row>
-    <row r="120" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="120" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A120" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C120" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D120" s="7">
         <v>0</v>
@@ -14463,15 +14497,15 @@
         <v>33120</v>
       </c>
     </row>
-    <row r="121" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="121" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A121" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C121" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D121" s="7">
         <v>0</v>
@@ -14576,15 +14610,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="122" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A122" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C122" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D122" s="7">
         <v>0</v>
@@ -14689,15 +14723,15 @@
         <v>183</v>
       </c>
     </row>
-    <row r="123" spans="1:37" x14ac:dyDescent="0.75">
+    <row r="123" spans="1:37" hidden="1" x14ac:dyDescent="0.75">
       <c r="A123" s="5" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C123" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D123" s="8">
         <v>0</v>
@@ -14803,6 +14837,15 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:AK123" xr:uid="{448F5820-9B09-4170-A743-862EF891E4AC}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="PT064"/>
+        <filter val="PT065"/>
+        <filter val="PT070"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>